<commit_message>
update TC4 & TD5
</commit_message>
<xml_diff>
--- a/MiddleAssignment_LeTuanSang/TestDesign5/TestDesign5_LeTuanSang.xlsx
+++ b/MiddleAssignment_LeTuanSang/TestDesign5/TestDesign5_LeTuanSang.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Downloads\NashTechHomeWork_LeTuanSang\MiddleAssignment_LeTuanSang\TestDesign5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\NashTechHomeWork_LeTuanSang\MiddleAssignment_LeTuanSang\TestCase5\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2223D06-686F-40C7-9882-2D54C84352C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Record of Change" sheetId="1" r:id="rId1"/>
@@ -37,14 +38,15 @@
     <definedName name="Result_CS_IT_1.1_004">#REF!</definedName>
     <definedName name="safa">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -55,12 +57,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -91,12 +93,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="G17" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -114,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -132,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G86" authorId="0" shapeId="0">
+    <comment ref="G86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G88" authorId="0" shapeId="0">
+    <comment ref="G88" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -200,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G91" authorId="0" shapeId="0">
+    <comment ref="G91" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G104" authorId="0" shapeId="0">
+    <comment ref="G104" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -250,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H104" authorId="0" shapeId="0">
+    <comment ref="H104" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
       <text>
         <r>
           <rPr>
@@ -275,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G105" authorId="0" shapeId="0">
+    <comment ref="G105" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -300,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H105" authorId="0" shapeId="0">
+    <comment ref="H105" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -325,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G110" authorId="0" shapeId="0">
+    <comment ref="G110" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -350,7 +352,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H110" authorId="0" shapeId="0">
+    <comment ref="H110" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -375,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G113" authorId="0" shapeId="0">
+    <comment ref="G113" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -400,7 +402,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G128" authorId="0" shapeId="0">
+    <comment ref="G128" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -425,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G130" authorId="0" shapeId="0">
+    <comment ref="G130" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -455,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="209">
   <si>
     <r>
       <rPr>
@@ -1163,41 +1165,42 @@
     <t>Verify pop-up is display when click on delete icon</t>
   </si>
   <si>
-    <t>Delete  Address successfully when Address is not default</t>
-  </si>
-  <si>
-    <t>Delete icon is clickable and Pop-up is displayed, title, content ( address, phone number, button</t>
-  </si>
-  <si>
-    <t>Delete Default Address unsuccsessfully</t>
-  </si>
-  <si>
     <t>Delete Address successfully when default address is change to normal address</t>
   </si>
   <si>
-    <t>Cannot delete address when click on x icon</t>
-  </si>
-  <si>
-    <t>Cannot delete address when click on cancel button</t>
-  </si>
-  <si>
-    <t>Cannot delete address when press ESC on keybroad</t>
-  </si>
-  <si>
-    <t>Address is deleted successfully. Close the pop-up. Deleted address is not displayed on Address Book</t>
-  </si>
-  <si>
-    <t>User cannot delete default address
-Error message "Error message: You cannot delete your default address" will be displayed if usertries to delete default address</t>
-  </si>
-  <si>
-    <t>toast message, auto close on 5s, or click x icon close</t>
+    <t xml:space="preserve">Delete non default Address successfully </t>
+  </si>
+  <si>
+    <t>Delete address fail when click on x icon</t>
+  </si>
+  <si>
+    <t>Delete address fail when click on cancel button</t>
+  </si>
+  <si>
+    <t>Delete address fail when press ESC on keybroad</t>
+  </si>
+  <si>
+    <t>Delete address fail, close pop-up, back to Edit My Address screen</t>
+  </si>
+  <si>
+    <t>- Address is deleted successfully. Close the pop-up.
+- Back to Address Book. Deleted address is not displayed on Address Book</t>
+  </si>
+  <si>
+    <t>Delete default Address fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Delete address fail, close pop-up, back to Edit My Address screen
+- A toast is displayed in the upper right corner with "Error message: You cannot delete your default address" </t>
+  </si>
+  <si>
+    <t>- Delete icon is clickable and Pop-up is displayed, title, content ( address, phone number, button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d&quot;, &quot;yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]General"/>
@@ -1205,7 +1208,7 @@
     <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="168" formatCode="[$-409]0.00%"/>
   </numFmts>
-  <fonts count="65">
+  <fonts count="68">
     <font>
       <sz val="11"/>
       <color rgb="FF323232"/>
@@ -1687,6 +1690,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="17">
     <fill>
@@ -2037,7 +2057,7 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="229">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
@@ -2543,6 +2563,28 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="14" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="65" fillId="15" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="14" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="14" borderId="13" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="15" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="15" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2666,42 +2708,38 @@
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="13" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="14" borderId="3" xfId="18" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="65" fillId="15" borderId="3" xfId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
-    <cellStyle name="background" xfId="2"/>
-    <cellStyle name="background 2" xfId="3"/>
-    <cellStyle name="body_tyext" xfId="4"/>
-    <cellStyle name="cell" xfId="5"/>
-    <cellStyle name="document title" xfId="6"/>
-    <cellStyle name="group" xfId="7"/>
-    <cellStyle name="Header" xfId="8"/>
-    <cellStyle name="Heading 3" xfId="9"/>
+    <cellStyle name="background" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="background 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="body_tyext" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="document title" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="group" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Header" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Heading 3" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="10"/>
+    <cellStyle name="Hyperlink 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="11"/>
-    <cellStyle name="Normal 2 2" xfId="12"/>
-    <cellStyle name="Normal 2 3" xfId="13"/>
-    <cellStyle name="Normal 3" xfId="14"/>
-    <cellStyle name="Normal 4" xfId="15"/>
-    <cellStyle name="Normal 6" xfId="16"/>
-    <cellStyle name="Normal_GUI - Checklist" xfId="17"/>
-    <cellStyle name="Normal_Sheet1" xfId="18"/>
-    <cellStyle name="page title" xfId="19"/>
-    <cellStyle name="Paragrap title" xfId="20"/>
-    <cellStyle name="Paragrap title 2" xfId="21"/>
-    <cellStyle name="Percent 2" xfId="22"/>
-    <cellStyle name="Table header" xfId="23"/>
-    <cellStyle name="Table header 2" xfId="24"/>
-    <cellStyle name="table_cell" xfId="25"/>
-    <cellStyle name="標準_040802 債権ＤＢ" xfId="26"/>
+    <cellStyle name="Normal 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 3" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 4" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 6" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal_GUI - Checklist" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="page title" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Paragrap title" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Paragrap title 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Percent 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Table header" xfId="23" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Table header 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="table_cell" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="標準_040802 債権ＤＢ" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2907,7 +2945,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="vi-VN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2931,8 +2969,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3107,7 +3151,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="vi-VN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3131,8 +3175,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3298,7 +3348,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="vi-VN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3322,8 +3372,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3332,8 +3388,17 @@
             <c:numRef>
               <c:f>'User Story 1'!$D$23:$D$76</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>@</c:formatCode>
                 <c:ptCount val="54"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3489,7 +3554,7 @@
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="vi-VN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3513,8 +3578,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3692,7 +3763,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="vi-VN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="86834804"/>
@@ -3740,7 +3811,7 @@
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="vi-VN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="47764545"/>
@@ -3775,7 +3846,7 @@
               <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="vi-VN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4235,7 +4306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ49"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -4282,37 +4353,37 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
-      <c r="A4" s="187" t="s">
+      <c r="A4" s="195" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="187"/>
-      <c r="C4" s="187"/>
-      <c r="D4" s="187"/>
-      <c r="E4" s="187"/>
+      <c r="B4" s="195"/>
+      <c r="C4" s="195"/>
+      <c r="D4" s="195"/>
+      <c r="E4" s="195"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A5" s="188" t="s">
+      <c r="A5" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="188"/>
-      <c r="C5" s="189" t="s">
+      <c r="B5" s="196"/>
+      <c r="C5" s="197" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="189"/>
-      <c r="E5" s="189"/>
+      <c r="D5" s="197"/>
+      <c r="E5" s="197"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="29.25" customHeight="1">
-      <c r="A6" s="190" t="s">
+      <c r="A6" s="198" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="190"/>
-      <c r="C6" s="186" t="s">
+      <c r="B6" s="198"/>
+      <c r="C6" s="194" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="29.25" customHeight="1">
@@ -4324,14 +4395,14 @@
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" ht="29.25" customHeight="1">
-      <c r="A8" s="185" t="s">
+      <c r="A8" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="185"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
+      <c r="B8" s="193"/>
+      <c r="C8" s="193"/>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="10" t="s">
@@ -4414,14 +4485,14 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="9" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="186" t="s">
+      <c r="A13" s="194" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="186"/>
-      <c r="C13" s="186"/>
-      <c r="D13" s="186"/>
-      <c r="E13" s="186"/>
-      <c r="F13" s="186"/>
+      <c r="B13" s="194"/>
+      <c r="C13" s="194"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="194"/>
+      <c r="F13" s="194"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="6"/>
@@ -4515,7 +4586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ33"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -4544,36 +4615,36 @@
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" customHeight="1">
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="203" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="195"/>
-      <c r="G2" s="195"/>
-      <c r="H2" s="195"/>
-      <c r="I2" s="195"/>
-      <c r="J2" s="196" t="s">
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="203"/>
+      <c r="H2" s="203"/>
+      <c r="I2" s="203"/>
+      <c r="J2" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="196"/>
+      <c r="K2" s="204"/>
     </row>
     <row r="3" spans="1:11" ht="28.5" customHeight="1">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="197"/>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="198" t="s">
+      <c r="C3" s="205"/>
+      <c r="D3" s="205"/>
+      <c r="E3" s="205"/>
+      <c r="F3" s="206" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="198"/>
-      <c r="H3" s="198"/>
-      <c r="I3" s="198"/>
-      <c r="J3" s="196"/>
-      <c r="K3" s="196"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="206"/>
+      <c r="I3" s="206"/>
+      <c r="J3" s="204"/>
+      <c r="K3" s="204"/>
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1">
       <c r="B4" s="26"/>
@@ -4593,65 +4664,65 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A7" s="193" t="s">
+      <c r="A7" s="201" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="193"/>
-      <c r="C7" s="193"/>
-      <c r="D7" s="193"/>
-      <c r="E7" s="193"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="193"/>
-      <c r="I7" s="193"/>
+      <c r="B7" s="201"/>
+      <c r="C7" s="201"/>
+      <c r="D7" s="201"/>
+      <c r="E7" s="201"/>
+      <c r="F7" s="201"/>
+      <c r="G7" s="201"/>
+      <c r="H7" s="201"/>
+      <c r="I7" s="201"/>
     </row>
     <row r="8" spans="1:11" ht="20.25" customHeight="1">
-      <c r="A8" s="193"/>
-      <c r="B8" s="193"/>
-      <c r="C8" s="193"/>
-      <c r="D8" s="193"/>
-      <c r="E8" s="193"/>
-      <c r="F8" s="193"/>
-      <c r="G8" s="193"/>
-      <c r="H8" s="193"/>
-      <c r="I8" s="193"/>
+      <c r="A8" s="201"/>
+      <c r="B8" s="201"/>
+      <c r="C8" s="201"/>
+      <c r="D8" s="201"/>
+      <c r="E8" s="201"/>
+      <c r="F8" s="201"/>
+      <c r="G8" s="201"/>
+      <c r="H8" s="201"/>
+      <c r="I8" s="201"/>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
+      <c r="B9" s="201"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="201"/>
     </row>
     <row r="10" spans="1:11" ht="21" customHeight="1">
-      <c r="A10" s="193"/>
-      <c r="B10" s="193"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
+      <c r="A10" s="201"/>
+      <c r="B10" s="201"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="201"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="194" t="s">
+      <c r="A11" s="202" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="194"/>
-      <c r="C11" s="194"/>
-      <c r="D11" s="194"/>
-      <c r="E11" s="194"/>
-      <c r="F11" s="194"/>
-      <c r="G11" s="194"/>
-      <c r="H11" s="194"/>
-      <c r="I11" s="194"/>
+      <c r="B11" s="202"/>
+      <c r="C11" s="202"/>
+      <c r="D11" s="202"/>
+      <c r="E11" s="202"/>
+      <c r="F11" s="202"/>
+      <c r="G11" s="202"/>
+      <c r="H11" s="202"/>
+      <c r="I11" s="202"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="30"/>
@@ -4673,65 +4744,65 @@
       <c r="A14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="191" t="s">
+      <c r="B14" s="199" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="191"/>
-      <c r="D14" s="191"/>
-      <c r="E14" s="191"/>
-      <c r="F14" s="191"/>
-      <c r="G14" s="191"/>
-      <c r="H14" s="191"/>
-      <c r="I14" s="191"/>
-      <c r="J14" s="191"/>
-      <c r="K14" s="191"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="199"/>
+      <c r="E14" s="199"/>
+      <c r="F14" s="199"/>
+      <c r="G14" s="199"/>
+      <c r="H14" s="199"/>
+      <c r="I14" s="199"/>
+      <c r="J14" s="199"/>
+      <c r="K14" s="199"/>
     </row>
     <row r="15" spans="1:11" ht="14.25" customHeight="1">
       <c r="A15" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="191" t="s">
+      <c r="B15" s="199" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="191"/>
-      <c r="D15" s="191"/>
-      <c r="E15" s="191"/>
-      <c r="F15" s="191"/>
-      <c r="G15" s="191"/>
-      <c r="H15" s="191"/>
-      <c r="I15" s="191"/>
-      <c r="J15" s="191"/>
-      <c r="K15" s="191"/>
+      <c r="C15" s="199"/>
+      <c r="D15" s="199"/>
+      <c r="E15" s="199"/>
+      <c r="F15" s="199"/>
+      <c r="G15" s="199"/>
+      <c r="H15" s="199"/>
+      <c r="I15" s="199"/>
+      <c r="J15" s="199"/>
+      <c r="K15" s="199"/>
     </row>
     <row r="16" spans="1:11" ht="14.25" customHeight="1">
       <c r="A16" s="31"/>
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="199" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="191"/>
-      <c r="D16" s="191"/>
-      <c r="E16" s="191"/>
-      <c r="F16" s="191"/>
-      <c r="G16" s="191"/>
-      <c r="H16" s="191"/>
-      <c r="I16" s="191"/>
-      <c r="J16" s="191"/>
-      <c r="K16" s="191"/>
+      <c r="C16" s="199"/>
+      <c r="D16" s="199"/>
+      <c r="E16" s="199"/>
+      <c r="F16" s="199"/>
+      <c r="G16" s="199"/>
+      <c r="H16" s="199"/>
+      <c r="I16" s="199"/>
+      <c r="J16" s="199"/>
+      <c r="K16" s="199"/>
     </row>
     <row r="17" spans="1:14" ht="14.25" customHeight="1">
       <c r="A17" s="31"/>
-      <c r="B17" s="191" t="s">
+      <c r="B17" s="199" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="191"/>
-      <c r="D17" s="191"/>
-      <c r="E17" s="191"/>
-      <c r="F17" s="191"/>
-      <c r="G17" s="191"/>
-      <c r="H17" s="191"/>
-      <c r="I17" s="191"/>
-      <c r="J17" s="191"/>
-      <c r="K17" s="191"/>
+      <c r="C17" s="199"/>
+      <c r="D17" s="199"/>
+      <c r="E17" s="199"/>
+      <c r="F17" s="199"/>
+      <c r="G17" s="199"/>
+      <c r="H17" s="199"/>
+      <c r="I17" s="199"/>
+      <c r="J17" s="199"/>
+      <c r="K17" s="199"/>
     </row>
     <row r="19" spans="1:14" ht="23.25">
       <c r="A19" s="29" t="s">
@@ -4742,40 +4813,40 @@
       <c r="A20" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="191" t="s">
+      <c r="B20" s="199" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="191"/>
-      <c r="D20" s="191"/>
-      <c r="E20" s="191"/>
-      <c r="F20" s="191"/>
-      <c r="G20" s="191"/>
+      <c r="C20" s="199"/>
+      <c r="D20" s="199"/>
+      <c r="E20" s="199"/>
+      <c r="F20" s="199"/>
+      <c r="G20" s="199"/>
     </row>
     <row r="21" spans="1:14" ht="12.75" customHeight="1">
       <c r="A21" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="199" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="191"/>
-      <c r="D21" s="191"/>
-      <c r="E21" s="191"/>
-      <c r="F21" s="191"/>
-      <c r="G21" s="191"/>
+      <c r="C21" s="199"/>
+      <c r="D21" s="199"/>
+      <c r="E21" s="199"/>
+      <c r="F21" s="199"/>
+      <c r="G21" s="199"/>
     </row>
     <row r="22" spans="1:14" ht="12.75" customHeight="1">
       <c r="A22" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="191" t="s">
+      <c r="B22" s="199" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="191"/>
-      <c r="D22" s="191"/>
-      <c r="E22" s="191"/>
-      <c r="F22" s="191"/>
-      <c r="G22" s="191"/>
+      <c r="C22" s="199"/>
+      <c r="D22" s="199"/>
+      <c r="E22" s="199"/>
+      <c r="F22" s="199"/>
+      <c r="G22" s="199"/>
     </row>
     <row r="24" spans="1:14" ht="23.25">
       <c r="A24" s="29" t="s">
@@ -4834,11 +4905,11 @@
       <c r="N27" s="34"/>
     </row>
     <row r="29" spans="1:14" ht="21.75" customHeight="1">
-      <c r="B29" s="192" t="s">
+      <c r="B29" s="200" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="192"/>
-      <c r="D29" s="192"/>
+      <c r="C29" s="200"/>
+      <c r="D29" s="200"/>
     </row>
     <row r="30" spans="1:14" ht="90" customHeight="1">
       <c r="B30" s="35"/>
@@ -4884,7 +4955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
@@ -4915,14 +4986,14 @@
       <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" s="40" customFormat="1" ht="25.5">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="207" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="199"/>
-      <c r="C2" s="199"/>
-      <c r="D2" s="199"/>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="41"/>
@@ -5076,7 +5147,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
@@ -5105,12 +5176,12 @@
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="26.25">
-      <c r="A2" s="200" t="s">
+      <c r="A2" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="200"/>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
+      <c r="B2" s="208"/>
+      <c r="C2" s="208"/>
+      <c r="D2" s="208"/>
       <c r="E2" s="55"/>
       <c r="F2" s="56"/>
       <c r="G2" s="56"/>
@@ -5271,18 +5342,18 @@
       <c r="F14" s="62"/>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1">
-      <c r="A16" s="201" t="s">
+      <c r="A16" s="209" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="201"/>
+      <c r="B16" s="209"/>
       <c r="C16" s="65"/>
       <c r="D16" s="66"/>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1">
-      <c r="A17" s="202" t="s">
+      <c r="A17" s="210" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="202"/>
+      <c r="B17" s="210"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="67"/>
@@ -5297,7 +5368,7 @@
     <mergeCell ref="A17:B17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D14" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Yes,No,NA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5309,7 +5380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5326,19 +5397,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ130"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.28515625" style="68" customWidth="1"/>
-    <col min="2" max="2" width="61.28515625" style="69" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" style="70" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" style="70" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="69" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="70" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="70" customWidth="1"/>
     <col min="5" max="5" width="64.28515625" style="70" customWidth="1"/>
     <col min="6" max="6" width="39.5703125" style="70" customWidth="1"/>
     <col min="7" max="9" width="9.7109375" style="70" customWidth="1"/>
@@ -5347,10 +5418,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="23" customFormat="1" ht="14.25">
-      <c r="A1" s="209"/>
-      <c r="B1" s="209"/>
-      <c r="C1" s="209"/>
-      <c r="D1" s="209"/>
+      <c r="A1" s="217"/>
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
       <c r="E1" s="25"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
@@ -5360,14 +5431,14 @@
       <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:25" s="23" customFormat="1" ht="26.25">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="211"/>
+      <c r="F2" s="219"/>
       <c r="G2" s="56"/>
       <c r="H2" s="56"/>
       <c r="I2" s="56"/>
@@ -5377,10 +5448,10 @@
     <row r="3" spans="1:25" s="23" customFormat="1" ht="23.25">
       <c r="A3" s="72"/>
       <c r="B3" s="73"/>
-      <c r="C3" s="212"/>
-      <c r="D3" s="212"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
       <c r="E3" s="74"/>
-      <c r="F3" s="211"/>
+      <c r="F3" s="219"/>
       <c r="G3" s="56"/>
       <c r="H3" s="56"/>
       <c r="I3" s="56"/>
@@ -5391,9 +5462,9 @@
       <c r="A4" s="75" t="s">
         <v>197</v>
       </c>
-      <c r="B4" s="206"/>
-      <c r="C4" s="206"/>
-      <c r="D4" s="206"/>
+      <c r="B4" s="214"/>
+      <c r="C4" s="214"/>
+      <c r="D4" s="214"/>
       <c r="E4" s="76"/>
       <c r="F4" s="77"/>
       <c r="G4" s="77"/>
@@ -5408,9 +5479,9 @@
       <c r="A5" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="206"/>
-      <c r="C5" s="206"/>
-      <c r="D5" s="206"/>
+      <c r="B5" s="214"/>
+      <c r="C5" s="214"/>
+      <c r="D5" s="214"/>
       <c r="E5" s="76"/>
       <c r="F5" s="77"/>
       <c r="G5" s="77"/>
@@ -5425,9 +5496,9 @@
       <c r="A6" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="206"/>
-      <c r="C6" s="206"/>
-      <c r="D6" s="206"/>
+      <c r="B6" s="214"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="214"/>
       <c r="E6" s="76"/>
       <c r="F6" s="77"/>
       <c r="G6" s="77"/>
@@ -5439,11 +5510,11 @@
       <c r="A7" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="206" t="s">
+      <c r="B7" s="214" t="s">
         <v>97</v>
       </c>
-      <c r="C7" s="206"/>
-      <c r="D7" s="206"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="214"/>
       <c r="E7" s="76"/>
       <c r="F7" s="77"/>
       <c r="G7" s="77"/>
@@ -5456,9 +5527,9 @@
       <c r="A8" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="207"/>
-      <c r="C8" s="207"/>
-      <c r="D8" s="207"/>
+      <c r="B8" s="215"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
       <c r="E8" s="82"/>
       <c r="F8" s="77"/>
     </row>
@@ -5610,11 +5681,11 @@
       <c r="D16" s="94"/>
       <c r="E16" s="94"/>
       <c r="F16" s="95"/>
-      <c r="G16" s="208" t="s">
+      <c r="G16" s="216" t="s">
         <v>99</v>
       </c>
-      <c r="H16" s="208"/>
-      <c r="I16" s="208"/>
+      <c r="H16" s="216"/>
+      <c r="I16" s="216"/>
       <c r="J16" s="96"/>
     </row>
     <row r="17" spans="1:11" s="97" customFormat="1">
@@ -5643,11 +5714,11 @@
     </row>
     <row r="18" spans="1:11" s="97" customFormat="1" ht="12.75">
       <c r="A18" s="183"/>
-      <c r="B18" s="204" t="s">
+      <c r="B18" s="212" t="s">
         <v>196</v>
       </c>
-      <c r="C18" s="204"/>
-      <c r="D18" s="204"/>
+      <c r="C18" s="212"/>
+      <c r="D18" s="212"/>
       <c r="E18" s="101"/>
       <c r="F18" s="100"/>
       <c r="G18" s="102"/>
@@ -5655,112 +5726,132 @@
       <c r="I18" s="102"/>
       <c r="J18" s="100"/>
     </row>
-    <row r="19" spans="1:11" s="97" customFormat="1" ht="25.5">
-      <c r="A19" s="183"/>
-      <c r="B19" s="177" t="s">
-        <v>199</v>
-      </c>
-      <c r="C19" s="178"/>
-      <c r="D19" s="171" t="s">
-        <v>206</v>
-      </c>
-      <c r="E19" s="226"/>
-      <c r="F19" s="178"/>
-      <c r="G19" s="227"/>
-      <c r="H19" s="227"/>
-      <c r="I19" s="227"/>
-      <c r="J19" s="178"/>
-    </row>
-    <row r="20" spans="1:11" s="103" customFormat="1" ht="38.25">
-      <c r="A20" s="182">
+    <row r="19" spans="1:11" s="103" customFormat="1" ht="25.5">
+      <c r="A19" s="185">
+        <v>1</v>
+      </c>
+      <c r="B19" s="188" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="191"/>
+      <c r="D19" s="234" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="188"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="171"/>
+      <c r="H19" s="171"/>
+      <c r="I19" s="171"/>
+      <c r="J19" s="172"/>
+    </row>
+    <row r="20" spans="1:11" s="97" customFormat="1" ht="51">
+      <c r="A20" s="183">
         <f ca="1">IF(OFFSET(A20,-1,0) ="",OFFSET(A20,-2,0)+1,OFFSET(A20,-1,0)+1 )</f>
-        <v>1</v>
-      </c>
-      <c r="B20" s="177" t="s">
-        <v>201</v>
-      </c>
-      <c r="C20" s="168"/>
-      <c r="D20" s="171" t="s">
-        <v>207</v>
-      </c>
-      <c r="E20" s="168"/>
-      <c r="F20" s="170"/>
-      <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
-      <c r="I20" s="171"/>
-      <c r="J20" s="172"/>
-    </row>
-    <row r="21" spans="1:11" s="103" customFormat="1" ht="25.5">
+        <v>2</v>
+      </c>
+      <c r="B20" s="188" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="189"/>
+      <c r="D20" s="234" t="s">
+        <v>205</v>
+      </c>
+      <c r="E20" s="190"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="186"/>
+      <c r="H20" s="186"/>
+      <c r="I20" s="186"/>
+      <c r="J20" s="178"/>
+    </row>
+    <row r="21" spans="1:11" s="103" customFormat="1" ht="63.75">
       <c r="A21" s="182">
         <f ca="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
-        <v>2</v>
-      </c>
-      <c r="B21" s="177" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="168"/>
-      <c r="D21" s="171" t="s">
-        <v>200</v>
-      </c>
-      <c r="E21" s="171" t="s">
-        <v>208</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B21" s="188" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="191"/>
+      <c r="D21" s="234" t="s">
+        <v>207</v>
+      </c>
+      <c r="E21" s="191"/>
       <c r="F21" s="170"/>
       <c r="G21" s="171"/>
       <c r="H21" s="171"/>
       <c r="I21" s="171"/>
       <c r="J21" s="172"/>
     </row>
-    <row r="22" spans="1:11" s="103" customFormat="1" ht="30">
-      <c r="A22" s="184"/>
-      <c r="B22" s="177" t="s">
-        <v>202</v>
-      </c>
-      <c r="C22" s="168"/>
-      <c r="D22" s="171"/>
-      <c r="E22" s="168"/>
+    <row r="22" spans="1:11" s="103" customFormat="1" ht="38.25">
+      <c r="A22" s="185">
+        <f t="shared" ref="A22:A25" ca="1" si="0">IF(OFFSET(A22,-1,0) ="",OFFSET(A22,-2,0)+1,OFFSET(A22,-1,0)+1 )</f>
+        <v>4</v>
+      </c>
+      <c r="B22" s="188" t="s">
+        <v>199</v>
+      </c>
+      <c r="C22" s="191"/>
+      <c r="D22" s="234" t="s">
+        <v>205</v>
+      </c>
+      <c r="E22" s="191"/>
       <c r="F22" s="170"/>
       <c r="G22" s="171"/>
       <c r="H22" s="171"/>
       <c r="I22" s="171"/>
       <c r="J22" s="172"/>
     </row>
-    <row r="23" spans="1:11" s="103" customFormat="1">
-      <c r="A23" s="184"/>
-      <c r="B23" s="177" t="s">
-        <v>203</v>
-      </c>
-      <c r="C23" s="168"/>
-      <c r="D23" s="168"/>
-      <c r="E23" s="168"/>
+    <row r="23" spans="1:11" s="103" customFormat="1" ht="25.5">
+      <c r="A23" s="185">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B23" s="188" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" s="191"/>
+      <c r="D23" s="234" t="s">
+        <v>204</v>
+      </c>
+      <c r="E23" s="191"/>
       <c r="F23" s="170"/>
       <c r="G23" s="171"/>
       <c r="H23" s="171"/>
       <c r="I23" s="171"/>
       <c r="J23" s="172"/>
     </row>
-    <row r="24" spans="1:11" s="103" customFormat="1">
-      <c r="A24" s="184"/>
-      <c r="B24" s="177" t="s">
+    <row r="24" spans="1:11" s="103" customFormat="1" ht="25.5">
+      <c r="A24" s="185">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B24" s="188" t="s">
+        <v>202</v>
+      </c>
+      <c r="C24" s="191"/>
+      <c r="D24" s="234" t="s">
         <v>204</v>
       </c>
-      <c r="C24" s="168"/>
-      <c r="D24" s="168"/>
-      <c r="E24" s="168"/>
+      <c r="E24" s="191"/>
       <c r="F24" s="170"/>
       <c r="G24" s="171"/>
       <c r="H24" s="171"/>
       <c r="I24" s="171"/>
       <c r="J24" s="172"/>
     </row>
-    <row r="25" spans="1:11" s="103" customFormat="1">
-      <c r="A25" s="184"/>
-      <c r="B25" s="177" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" s="168"/>
-      <c r="D25" s="168"/>
-      <c r="E25" s="168"/>
+    <row r="25" spans="1:11" s="103" customFormat="1" ht="25.5">
+      <c r="A25" s="185">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B25" s="188" t="s">
+        <v>203</v>
+      </c>
+      <c r="C25" s="191"/>
+      <c r="D25" s="234" t="s">
+        <v>204</v>
+      </c>
+      <c r="E25" s="191"/>
       <c r="F25" s="170"/>
       <c r="G25" s="171"/>
       <c r="H25" s="171"/>
@@ -5769,10 +5860,10 @@
     </row>
     <row r="26" spans="1:11" s="103" customFormat="1">
       <c r="A26" s="184"/>
-      <c r="B26" s="177"/>
-      <c r="C26" s="168"/>
-      <c r="D26" s="168"/>
-      <c r="E26" s="168"/>
+      <c r="B26" s="192"/>
+      <c r="C26" s="191"/>
+      <c r="D26" s="191"/>
+      <c r="E26" s="191"/>
       <c r="F26" s="170"/>
       <c r="G26" s="171"/>
       <c r="H26" s="171"/>
@@ -5780,13 +5871,10 @@
       <c r="J26" s="172"/>
     </row>
     <row r="27" spans="1:11" s="103" customFormat="1" ht="14.25">
-      <c r="A27" s="182">
-        <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
-        <v>1</v>
-      </c>
-      <c r="B27" s="228"/>
+      <c r="A27" s="182"/>
+      <c r="B27" s="187"/>
       <c r="C27" s="168"/>
-      <c r="D27" s="228"/>
+      <c r="D27" s="187"/>
       <c r="E27" s="168"/>
       <c r="F27" s="170"/>
       <c r="G27" s="171"/>
@@ -6492,9 +6580,9 @@
     </row>
     <row r="82" spans="1:10" s="107" customFormat="1">
       <c r="A82" s="105"/>
-      <c r="B82" s="205"/>
-      <c r="C82" s="205"/>
-      <c r="D82" s="205"/>
+      <c r="B82" s="213"/>
+      <c r="C82" s="213"/>
+      <c r="D82" s="213"/>
       <c r="E82" s="180"/>
       <c r="F82" s="170"/>
       <c r="G82" s="171"/>
@@ -6876,9 +6964,9 @@
     </row>
     <row r="114" spans="1:10" s="107" customFormat="1" ht="14.25">
       <c r="A114" s="109"/>
-      <c r="B114" s="203"/>
-      <c r="C114" s="203"/>
-      <c r="D114" s="203"/>
+      <c r="B114" s="211"/>
+      <c r="C114" s="211"/>
+      <c r="D114" s="211"/>
       <c r="E114" s="181"/>
       <c r="F114" s="175"/>
       <c r="G114" s="176"/>
@@ -6924,9 +7012,9 @@
     </row>
     <row r="118" spans="1:10" s="107" customFormat="1" ht="14.25">
       <c r="A118" s="109"/>
-      <c r="B118" s="203"/>
-      <c r="C118" s="203"/>
-      <c r="D118" s="203"/>
+      <c r="B118" s="211"/>
+      <c r="C118" s="211"/>
+      <c r="D118" s="211"/>
       <c r="E118" s="181"/>
       <c r="F118" s="175"/>
       <c r="G118" s="176"/>
@@ -6972,9 +7060,9 @@
     </row>
     <row r="122" spans="1:10" s="107" customFormat="1" ht="14.25">
       <c r="A122" s="109"/>
-      <c r="B122" s="203"/>
-      <c r="C122" s="203"/>
-      <c r="D122" s="203"/>
+      <c r="B122" s="211"/>
+      <c r="C122" s="211"/>
+      <c r="D122" s="211"/>
       <c r="E122" s="181"/>
       <c r="F122" s="175"/>
       <c r="G122" s="176"/>
@@ -7008,9 +7096,9 @@
     </row>
     <row r="125" spans="1:10" s="107" customFormat="1" ht="14.25">
       <c r="A125" s="109"/>
-      <c r="B125" s="203"/>
-      <c r="C125" s="203"/>
-      <c r="D125" s="203"/>
+      <c r="B125" s="211"/>
+      <c r="C125" s="211"/>
+      <c r="D125" s="211"/>
       <c r="E125" s="181"/>
       <c r="F125" s="175"/>
       <c r="G125" s="176"/>
@@ -7098,19 +7186,19 @@
     <mergeCell ref="B122:D122"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation showDropDown="1" showErrorMessage="1" sqref="G16:I17">
+    <dataValidation showDropDown="1" showErrorMessage="1" sqref="G16:I17" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18:I19">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18:I20" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G131:I188">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G131:I188" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G76:I130 H28:J75 G20:I27">
+    <dataValidation type="list" allowBlank="1" sqref="G76:I130 H28:J75 G19:I19 G21:I27" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>$A$11:$A$15</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7122,7 +7210,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7159,13 +7247,13 @@
     </row>
     <row r="2" spans="1:12" s="115" customFormat="1" ht="26.25">
       <c r="A2" s="114"/>
-      <c r="C2" s="223" t="s">
+      <c r="C2" s="231" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
-      <c r="G2" s="223"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
+      <c r="F2" s="231"/>
+      <c r="G2" s="231"/>
       <c r="H2" s="116" t="s">
         <v>110</v>
       </c>
@@ -7176,15 +7264,15 @@
     </row>
     <row r="3" spans="1:12" s="115" customFormat="1" ht="23.25">
       <c r="A3" s="114"/>
-      <c r="C3" s="224" t="s">
+      <c r="C3" s="232" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="224"/>
+      <c r="D3" s="232"/>
       <c r="E3" s="118"/>
-      <c r="F3" s="225" t="s">
+      <c r="F3" s="233" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="225"/>
+      <c r="G3" s="233"/>
       <c r="H3" s="117"/>
       <c r="I3" s="117"/>
       <c r="J3" s="119"/>
@@ -7209,10 +7297,10 @@
       <c r="L5" s="124"/>
     </row>
     <row r="6" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B6" s="219" t="s">
+      <c r="B6" s="227" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="219"/>
+      <c r="C6" s="227"/>
       <c r="D6" s="126"/>
       <c r="E6" s="126"/>
       <c r="F6" s="126"/>
@@ -7381,11 +7469,11 @@
       <c r="G13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B14" s="219" t="s">
+      <c r="B14" s="227" t="s">
         <v>143</v>
       </c>
-      <c r="C14" s="219"/>
-      <c r="D14" s="219"/>
+      <c r="C14" s="227"/>
+      <c r="D14" s="227"/>
       <c r="E14" s="126"/>
       <c r="F14" s="126"/>
       <c r="G14" s="127"/>
@@ -7561,11 +7649,11 @@
       <c r="G22" s="130"/>
     </row>
     <row r="23" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B23" s="219" t="s">
+      <c r="B23" s="227" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="219"/>
-      <c r="D23" s="219"/>
+      <c r="C23" s="227"/>
+      <c r="D23" s="227"/>
       <c r="E23" s="126"/>
       <c r="F23" s="126"/>
       <c r="G23" s="127"/>
@@ -7611,10 +7699,10 @@
       <c r="F26" s="132" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="222" t="s">
+      <c r="G26" s="230" t="s">
         <v>107</v>
       </c>
-      <c r="H26" s="222"/>
+      <c r="H26" s="230"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="139">
@@ -7639,8 +7727,8 @@
         <f>COUNTIFS(#REF!, "*Critical*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Critical*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
+      <c r="G27" s="228"/>
+      <c r="H27" s="228"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="139">
@@ -7665,8 +7753,8 @@
         <f>COUNTIFS(#REF!, "*Major*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Major*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G28" s="220"/>
-      <c r="H28" s="220"/>
+      <c r="G28" s="228"/>
+      <c r="H28" s="228"/>
     </row>
     <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="139">
@@ -7691,8 +7779,8 @@
         <f>COUNTIFS(#REF!, "*Normal*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Normal*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G29" s="220"/>
-      <c r="H29" s="220"/>
+      <c r="G29" s="228"/>
+      <c r="H29" s="228"/>
     </row>
     <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="139">
@@ -7717,8 +7805,8 @@
         <f>COUNTIFS(#REF!, "*Minor*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Minor*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G30" s="220"/>
-      <c r="H30" s="220"/>
+      <c r="G30" s="228"/>
+      <c r="H30" s="228"/>
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="139"/>
@@ -7739,8 +7827,8 @@
         <f>SUM(F27:F30)</f>
         <v>#REF!</v>
       </c>
-      <c r="G31" s="220"/>
-      <c r="H31" s="220"/>
+      <c r="G31" s="228"/>
+      <c r="H31" s="228"/>
     </row>
     <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="145"/>
@@ -7778,10 +7866,10 @@
       <c r="E34" s="132" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="216" t="s">
+      <c r="F34" s="224" t="s">
         <v>122</v>
       </c>
-      <c r="G34" s="216"/>
+      <c r="G34" s="224"/>
     </row>
     <row r="35" spans="1:12" s="138" customFormat="1" ht="14.25">
       <c r="A35" s="134"/>
@@ -7797,8 +7885,8 @@
       <c r="E35" s="143" t="s">
         <v>127</v>
       </c>
-      <c r="F35" s="221"/>
-      <c r="G35" s="221"/>
+      <c r="F35" s="229"/>
+      <c r="G35" s="229"/>
       <c r="H35" s="137"/>
       <c r="I35" s="137"/>
       <c r="J35" s="137"/>
@@ -7821,8 +7909,8 @@
       <c r="E36" s="144" t="s">
         <v>133</v>
       </c>
-      <c r="F36" s="220"/>
-      <c r="G36" s="220"/>
+      <c r="F36" s="228"/>
+      <c r="G36" s="228"/>
     </row>
     <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="139">
@@ -7840,8 +7928,8 @@
       <c r="E37" s="144" t="s">
         <v>133</v>
       </c>
-      <c r="F37" s="220"/>
-      <c r="G37" s="220"/>
+      <c r="F37" s="228"/>
+      <c r="G37" s="228"/>
     </row>
     <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="145"/>
@@ -7854,10 +7942,10 @@
       <c r="H38" s="149"/>
     </row>
     <row r="39" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B39" s="219" t="s">
+      <c r="B39" s="227" t="s">
         <v>176</v>
       </c>
-      <c r="C39" s="219"/>
+      <c r="C39" s="227"/>
       <c r="D39" s="126"/>
       <c r="E39" s="126"/>
       <c r="F39" s="126"/>
@@ -7881,15 +7969,15 @@
       <c r="B41" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="216" t="s">
+      <c r="C41" s="224" t="s">
         <v>178</v>
       </c>
-      <c r="D41" s="216"/>
-      <c r="E41" s="216" t="s">
+      <c r="D41" s="224"/>
+      <c r="E41" s="224" t="s">
         <v>179</v>
       </c>
-      <c r="F41" s="216"/>
-      <c r="G41" s="216"/>
+      <c r="F41" s="224"/>
+      <c r="G41" s="224"/>
       <c r="H41" s="131" t="s">
         <v>180</v>
       </c>
@@ -7901,15 +7989,15 @@
       <c r="B42" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="218" t="s">
+      <c r="C42" s="226" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="218"/>
-      <c r="E42" s="218" t="s">
+      <c r="D42" s="226"/>
+      <c r="E42" s="226" t="s">
         <v>183</v>
       </c>
-      <c r="F42" s="218"/>
-      <c r="G42" s="218"/>
+      <c r="F42" s="226"/>
+      <c r="G42" s="226"/>
       <c r="H42" s="154"/>
     </row>
     <row r="43" spans="1:12" ht="34.5" customHeight="1">
@@ -7919,15 +8007,15 @@
       <c r="B43" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C43" s="218" t="s">
+      <c r="C43" s="226" t="s">
         <v>182</v>
       </c>
-      <c r="D43" s="218"/>
-      <c r="E43" s="218" t="s">
+      <c r="D43" s="226"/>
+      <c r="E43" s="226" t="s">
         <v>183</v>
       </c>
-      <c r="F43" s="218"/>
-      <c r="G43" s="218"/>
+      <c r="F43" s="226"/>
+      <c r="G43" s="226"/>
       <c r="H43" s="154"/>
     </row>
     <row r="44" spans="1:12" ht="34.5" customHeight="1">
@@ -7937,15 +8025,15 @@
       <c r="B44" s="153" t="s">
         <v>181</v>
       </c>
-      <c r="C44" s="218" t="s">
+      <c r="C44" s="226" t="s">
         <v>182</v>
       </c>
-      <c r="D44" s="218"/>
-      <c r="E44" s="218" t="s">
+      <c r="D44" s="226"/>
+      <c r="E44" s="226" t="s">
         <v>183</v>
       </c>
-      <c r="F44" s="218"/>
-      <c r="G44" s="218"/>
+      <c r="F44" s="226"/>
+      <c r="G44" s="226"/>
       <c r="H44" s="154"/>
     </row>
     <row r="45" spans="1:12">
@@ -7957,10 +8045,10 @@
       <c r="G45" s="130"/>
     </row>
     <row r="46" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B46" s="219" t="s">
+      <c r="B46" s="227" t="s">
         <v>184</v>
       </c>
-      <c r="C46" s="219"/>
+      <c r="C46" s="227"/>
       <c r="D46" s="126"/>
       <c r="E46" s="126"/>
       <c r="F46" s="126"/>
@@ -7978,25 +8066,25 @@
       <c r="G47" s="130"/>
     </row>
     <row r="48" spans="1:12" s="158" customFormat="1" ht="21" customHeight="1">
-      <c r="A48" s="214" t="s">
+      <c r="A48" s="222" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="215" t="s">
+      <c r="B48" s="223" t="s">
         <v>186</v>
       </c>
-      <c r="C48" s="216" t="s">
+      <c r="C48" s="224" t="s">
         <v>187</v>
       </c>
-      <c r="D48" s="216"/>
-      <c r="E48" s="216"/>
-      <c r="F48" s="216"/>
-      <c r="G48" s="217" t="s">
+      <c r="D48" s="224"/>
+      <c r="E48" s="224"/>
+      <c r="F48" s="224"/>
+      <c r="G48" s="225" t="s">
         <v>152</v>
       </c>
-      <c r="H48" s="217" t="s">
+      <c r="H48" s="225" t="s">
         <v>186</v>
       </c>
-      <c r="I48" s="213" t="s">
+      <c r="I48" s="221" t="s">
         <v>188</v>
       </c>
       <c r="J48" s="157"/>
@@ -8004,8 +8092,8 @@
       <c r="L48" s="157"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="214"/>
-      <c r="B49" s="215"/>
+      <c r="A49" s="222"/>
+      <c r="B49" s="223"/>
       <c r="C49" s="159" t="s">
         <v>161</v>
       </c>
@@ -8018,13 +8106,13 @@
       <c r="F49" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="G49" s="217"/>
-      <c r="H49" s="217"/>
-      <c r="I49" s="213"/>
+      <c r="G49" s="225"/>
+      <c r="H49" s="225"/>
+      <c r="I49" s="221"/>
     </row>
     <row r="50" spans="1:9" ht="38.25">
-      <c r="A50" s="214"/>
-      <c r="B50" s="215"/>
+      <c r="A50" s="222"/>
+      <c r="B50" s="223"/>
       <c r="C50" s="161" t="s">
         <v>189</v>
       </c>
@@ -8194,7 +8282,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:I52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H51:I52" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"PASS,FAIL"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>